<commit_message>
Updated 4 test data sheet
</commit_message>
<xml_diff>
--- a/Test Data/TC_143_Verify_Maximum_Battery_Standby_And_Battery_Alarm_Limits.xlsx
+++ b/Test Data/TC_143_Verify_Maximum_Battery_Standby_And_Battery_Alarm_Limits.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhasip\Desktop\NGConsys Automation_01_02_2019\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F6D5B9-E563-43DC-9928-1B439C3EF525}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="8" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Color Codes</t>
   </si>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,11 +522,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,13 +659,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>26</v>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>13</v>
@@ -673,32 +674,9 @@
         <v>16</v>
       </c>
       <c r="F10" s="11">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="G10" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5">
-        <v>16</v>
-      </c>
-      <c r="F11" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="G11" s="11">
         <v>5</v>
       </c>
     </row>
@@ -708,11 +686,12 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated test data for 5,24,40V,BatteryStandby and AC Calculations test cases
</commit_message>
<xml_diff>
--- a/Test Data/TC_143_Verify_Maximum_Battery_Standby_And_Battery_Alarm_Limits.xlsx
+++ b/Test Data/TC_143_Verify_Maximum_Battery_Standby_And_Battery_Alarm_Limits.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB505AB-D4BF-49AC-8541-7257A5E2CF65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="8" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Color Codes</t>
   </si>
@@ -120,9 +121,6 @@
     <t>Expected Max Battery Alarm Limits</t>
   </si>
   <si>
-    <t xml:space="preserve">NGC-488 </t>
-  </si>
-  <si>
     <t>AlarmLoadingDetail</t>
   </si>
   <si>
@@ -133,12 +131,18 @@
   </si>
   <si>
     <t>Alarm Current(A)</t>
+  </si>
+  <si>
+    <t>3.000</t>
+  </si>
+  <si>
+    <t>NGC-488/T381 OR TC-143</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,10 +246,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -533,11 +537,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,8 +591,8 @@
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>31</v>
+      <c r="B4" t="s">
+        <v>36</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="7" t="s">
@@ -624,10 +628,10 @@
         <v>30</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -637,7 +641,7 @@
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -646,17 +650,17 @@
       <c r="E8" s="5">
         <v>16</v>
       </c>
-      <c r="F8" s="11">
-        <v>3</v>
-      </c>
-      <c r="G8" s="11">
-        <v>5</v>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -666,8 +670,8 @@
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>15</v>
+      <c r="C9" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>13</v>
@@ -675,17 +679,17 @@
       <c r="E9" s="5">
         <v>16</v>
       </c>
-      <c r="F9" s="11">
-        <v>1.9</v>
-      </c>
-      <c r="G9" s="11">
-        <v>2.5</v>
+      <c r="F9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -695,8 +699,8 @@
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>15</v>
+      <c r="C10" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>13</v>
@@ -704,17 +708,17 @@
       <c r="E10" s="5">
         <v>16</v>
       </c>
-      <c r="F10" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="G10" s="11">
-        <v>5</v>
+      <c r="F10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>